<commit_message>
Correciones de menu principal
</commit_message>
<xml_diff>
--- a/Diseño de base de datos/diseño.xlsx
+++ b/Diseño de base de datos/diseño.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B629858-B248-4AEB-B3F8-D7025A9A3D67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF887475-3590-4365-886A-18F4A0C91AC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacional" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="200">
   <si>
     <t>Paciente</t>
   </si>
@@ -408,15 +408,6 @@
   </si>
   <si>
     <t>comentario JSON formato</t>
-  </si>
-  <si>
-    <t>{
-	idConsulta:
-	{
-		fecha:"fecha"
-		idDoctor:"comentario"
-	}	
-}</t>
   </si>
   <si>
     <t>ResultadosLab JSON formato</t>
@@ -650,7 +641,19 @@
     <t>Sarampión/Paperas/Rubeola (SPR)</t>
   </si>
   <si>
-    <t>correo</t>
+    <t>"CUI":20,
+{
+	idConsulta :
+	{
+		"Doctor1" : "Comentario",
+		"Doctor2" : "Comentario2",
+	},
+	idConsulta :
+	{
+		"Doctor2" : "Este cerote está que se muere juasjuas",
+		"Doctor1" : "Que feo este trabajo"
+	}
+}</t>
   </si>
 </sst>
 </file>
@@ -777,11 +780,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1065,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BM58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="X1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
@@ -1118,26 +1121,26 @@
         <v>19</v>
       </c>
       <c r="G2" s="19"/>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="K2" s="21"/>
+      <c r="N2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="O2" s="21"/>
+      <c r="R2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="20"/>
+      <c r="S2" s="21"/>
       <c r="V2" s="19" t="s">
         <v>28</v>
       </c>
       <c r="W2" s="19"/>
-      <c r="Z2" s="20" t="s">
+      <c r="Z2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="20"/>
+      <c r="AA2" s="21"/>
       <c r="AC2" s="19" t="s">
         <v>58</v>
       </c>
@@ -1146,14 +1149,14 @@
         <v>42</v>
       </c>
       <c r="AG2" s="19"/>
-      <c r="AJ2" s="20" t="s">
+      <c r="AJ2" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AK2" s="20"/>
-      <c r="AN2" s="20" t="s">
+      <c r="AK2" s="21"/>
+      <c r="AN2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AO2" s="20"/>
+      <c r="AO2" s="21"/>
       <c r="AR2" s="19" t="s">
         <v>46</v>
       </c>
@@ -1175,7 +1178,7 @@
       </c>
       <c r="BI2" s="19"/>
       <c r="BK2" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BL2" s="19"/>
     </row>
@@ -1335,25 +1338,25 @@
         <v>103</v>
       </c>
       <c r="AR4" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="AS4" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV4" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="AS4" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV4" s="16" t="s">
+      <c r="AW4" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ4" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="AW4" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ4" s="8" t="s">
+      <c r="BA4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="BD4" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="BA4" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="BD4" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="BE4" s="8" t="s">
         <v>98</v>
@@ -1379,7 +1382,7 @@
         <v>99</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>98</v>
@@ -1457,7 +1460,7 @@
         <v>97</v>
       </c>
       <c r="BK5" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BL5" s="4" t="s">
         <v>103</v>
@@ -1471,7 +1474,7 @@
         <v>97</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>98</v>
@@ -1554,7 +1557,7 @@
         <v>98</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>98</v>
@@ -1623,7 +1626,7 @@
         <v>96</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>98</v>
@@ -1694,7 +1697,7 @@
         <v>96</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>98</v>
@@ -1750,7 +1753,7 @@
         <v>98</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>98</v>
@@ -1761,18 +1764,16 @@
       <c r="W10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AC10" s="8" t="s">
-        <v>200</v>
-      </c>
+      <c r="AC10" s="8"/>
       <c r="AD10" s="4" t="s">
         <v>114</v>
       </c>
       <c r="AG10" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AH10" s="19"/>
       <c r="AK10" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AL10" s="19"/>
       <c r="AV10" s="7" t="s">
@@ -1794,7 +1795,7 @@
         <v>98</v>
       </c>
       <c r="BK10" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BL10" s="4" t="s">
         <v>103</v>
@@ -1808,7 +1809,7 @@
         <v>98</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>98</v>
@@ -1832,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="AQ11" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AR11" s="19"/>
       <c r="AV11" s="7" t="s">
@@ -1848,7 +1849,7 @@
         <v>116</v>
       </c>
       <c r="BC11" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BD11" s="19"/>
       <c r="BH11" s="9" t="s">
@@ -1866,7 +1867,7 @@
         <v>103</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>98</v>
@@ -1891,7 +1892,7 @@
         <v>64</v>
       </c>
       <c r="AW12" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AZ12" s="9" t="s">
         <v>76</v>
@@ -1942,7 +1943,7 @@
       </c>
       <c r="AA13" s="19"/>
       <c r="AD13" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AE13" s="19"/>
       <c r="AG13" s="8" t="s">
@@ -1967,7 +1968,7 @@
         <v>65</v>
       </c>
       <c r="AW13" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AZ13" s="9" t="s">
         <v>77</v>
@@ -2048,7 +2049,7 @@
         <v>105</v>
       </c>
       <c r="AQ14" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AR14" s="4" t="s">
         <v>103</v>
@@ -2066,7 +2067,7 @@
         <v>98</v>
       </c>
       <c r="BC14" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BD14" s="4" t="s">
         <v>103</v>
@@ -2140,7 +2141,7 @@
         <v>98</v>
       </c>
       <c r="BH15" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BI15" s="18" t="s">
         <v>98</v>
@@ -2216,7 +2217,7 @@
         <v>98</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>101</v>
@@ -2228,7 +2229,7 @@
         <v>104</v>
       </c>
       <c r="AD17" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AE17" s="4" t="s">
         <v>103</v>
@@ -2280,7 +2281,7 @@
       </c>
       <c r="AA18" s="19"/>
       <c r="AD18" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AE18" s="4" t="s">
         <v>103</v>
@@ -2342,13 +2343,13 @@
         <v>2</v>
       </c>
       <c r="AD19" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE19" s="4" t="s">
         <v>103</v>
       </c>
       <c r="AV19" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AW19" s="4" t="s">
         <v>114</v>
@@ -2392,7 +2393,7 @@
       </c>
       <c r="O20" s="19"/>
       <c r="V20" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W20" s="14" t="s">
         <v>121</v>
@@ -2404,7 +2405,7 @@
         <v>98</v>
       </c>
       <c r="AD20" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE20" s="4" t="s">
         <v>103</v>
@@ -2416,25 +2417,25 @@
         <v>114</v>
       </c>
       <c r="BC20" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BD20" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BF20" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG20" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BI20" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BJ20" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BL20" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BM20" s="4" t="s">
         <v>103</v>
@@ -2451,10 +2452,10 @@
         <v>106</v>
       </c>
       <c r="G21" s="19"/>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="K21" s="21"/>
+      <c r="K21" s="20"/>
       <c r="N21" s="3" t="s">
         <v>1</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="V21" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W21" s="14" t="s">
         <v>121</v>
@@ -2474,17 +2475,17 @@
         <v>121</v>
       </c>
       <c r="AD21" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE21" s="4" t="s">
         <v>103</v>
       </c>
       <c r="AK21" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AL21" s="19"/>
       <c r="AZ21" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BA21" s="4" t="s">
         <v>114</v>
@@ -2522,7 +2523,7 @@
         <v>121</v>
       </c>
       <c r="AD22" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AE22" s="4" t="s">
         <v>103</v>
@@ -2566,7 +2567,7 @@
         <v>101</v>
       </c>
       <c r="AD23" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AE23" s="4" t="s">
         <v>103</v>
@@ -2604,7 +2605,7 @@
         <v>101</v>
       </c>
       <c r="AD24" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AE24" s="4" t="s">
         <v>103</v>
@@ -2630,25 +2631,25 @@
     </row>
     <row r="25" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD25" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AE25" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BC25" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BD25" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BG25" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BH25" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BJ25" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BK25" s="4" t="s">
         <v>103</v>
@@ -2656,7 +2657,7 @@
     </row>
     <row r="26" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD26" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AE26" s="4" t="s">
         <v>103</v>
@@ -2664,7 +2665,7 @@
     </row>
     <row r="27" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD27" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AE27" s="4" t="s">
         <v>103</v>
@@ -2672,7 +2673,7 @@
     </row>
     <row r="28" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD28" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AE28" s="4" t="s">
         <v>103</v>
@@ -2680,7 +2681,7 @@
     </row>
     <row r="29" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD29" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AE29" s="4" t="s">
         <v>103</v>
@@ -2688,7 +2689,7 @@
     </row>
     <row r="30" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD30" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AE30" s="4" t="s">
         <v>103</v>
@@ -2696,7 +2697,7 @@
     </row>
     <row r="31" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD31" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AE31" s="4" t="s">
         <v>103</v>
@@ -2704,7 +2705,7 @@
     </row>
     <row r="32" spans="2:65" x14ac:dyDescent="0.25">
       <c r="AD32" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE32" s="4" t="s">
         <v>103</v>
@@ -2712,7 +2713,7 @@
     </row>
     <row r="33" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD33" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AE33" s="4" t="s">
         <v>103</v>
@@ -2720,7 +2721,7 @@
     </row>
     <row r="34" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD34" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AE34" s="4" t="s">
         <v>103</v>
@@ -2728,7 +2729,7 @@
     </row>
     <row r="35" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD35" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE35" s="4" t="s">
         <v>103</v>
@@ -2736,7 +2737,7 @@
     </row>
     <row r="36" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD36" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AE36" s="4" t="s">
         <v>103</v>
@@ -2744,7 +2745,7 @@
     </row>
     <row r="37" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD37" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE37" s="4" t="s">
         <v>103</v>
@@ -2752,7 +2753,7 @@
     </row>
     <row r="38" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD38" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE38" s="4" t="s">
         <v>103</v>
@@ -2760,7 +2761,7 @@
     </row>
     <row r="39" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD39" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AE39" s="4" t="s">
         <v>103</v>
@@ -2768,7 +2769,7 @@
     </row>
     <row r="40" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD40" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AE40" s="4" t="s">
         <v>103</v>
@@ -2776,7 +2777,7 @@
     </row>
     <row r="41" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD41" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AE41" s="4" t="s">
         <v>103</v>
@@ -2784,7 +2785,7 @@
     </row>
     <row r="42" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD42" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AE42" s="4" t="s">
         <v>103</v>
@@ -2792,7 +2793,7 @@
     </row>
     <row r="43" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD43" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AE43" s="4" t="s">
         <v>103</v>
@@ -2800,7 +2801,7 @@
     </row>
     <row r="44" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD44" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AE44" s="4" t="s">
         <v>103</v>
@@ -2808,7 +2809,7 @@
     </row>
     <row r="45" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD45" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE45" s="4" t="s">
         <v>103</v>
@@ -2816,7 +2817,7 @@
     </row>
     <row r="46" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD46" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AE46" s="4" t="s">
         <v>103</v>
@@ -2824,7 +2825,7 @@
     </row>
     <row r="47" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD47" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AE47" s="4" t="s">
         <v>103</v>
@@ -2832,7 +2833,7 @@
     </row>
     <row r="48" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD48" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AE48" s="4" t="s">
         <v>103</v>
@@ -2840,7 +2841,7 @@
     </row>
     <row r="49" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD49" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AE49" s="4" t="s">
         <v>103</v>
@@ -2848,7 +2849,7 @@
     </row>
     <row r="50" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD50" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AE50" s="4" t="s">
         <v>103</v>
@@ -2856,7 +2857,7 @@
     </row>
     <row r="51" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD51" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AE51" s="4" t="s">
         <v>103</v>
@@ -2864,7 +2865,7 @@
     </row>
     <row r="52" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD52" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AE52" s="4" t="s">
         <v>103</v>
@@ -2872,7 +2873,7 @@
     </row>
     <row r="53" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD53" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AE53" s="4" t="s">
         <v>103</v>
@@ -2888,7 +2889,7 @@
     </row>
     <row r="55" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD55" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AE55" s="4" t="s">
         <v>103</v>
@@ -2904,7 +2905,7 @@
     </row>
     <row r="57" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD57" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AE57" s="4" t="s">
         <v>116</v>
@@ -2912,7 +2913,7 @@
     </row>
     <row r="58" spans="30:31" x14ac:dyDescent="0.25">
       <c r="AD58" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AE58" s="4" t="s">
         <v>116</v>
@@ -2920,32 +2921,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="AK21:AL21"/>
-    <mergeCell ref="BC22:BD22"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="BG22:BH22"/>
-    <mergeCell ref="BJ22:BK22"/>
-    <mergeCell ref="BC17:BD17"/>
-    <mergeCell ref="BF17:BG17"/>
-    <mergeCell ref="BI17:BJ17"/>
-    <mergeCell ref="BL17:BM17"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="R2:S2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="AC2:AD2"/>
@@ -2960,6 +2935,32 @@
     <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="BC11:BD11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="BC22:BD22"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="BK7:BL7"/>
+    <mergeCell ref="BG22:BH22"/>
+    <mergeCell ref="BJ22:BK22"/>
+    <mergeCell ref="BC17:BD17"/>
+    <mergeCell ref="BF17:BG17"/>
+    <mergeCell ref="BI17:BJ17"/>
+    <mergeCell ref="BL17:BM17"/>
+    <mergeCell ref="BH2:BI2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2970,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76854342-D8FC-49A1-BF1E-FCE8D71C0819}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,12 +2988,12 @@
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D2" s="10"/>
       <c r="E2" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="E3" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -3008,13 +3009,13 @@
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="E6" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -3032,27 +3033,27 @@
         <v>126</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I12" s="12" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de disenio de BD
</commit_message>
<xml_diff>
--- a/Diseño de base de datos/diseño.xlsx
+++ b/Diseño de base de datos/diseño.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB2C48A-9766-4506-89AD-A980A49E75E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F8B234-7447-4119-BD46-F47CAB863A92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacional" sheetId="1" r:id="rId1"/>
     <sheet name="Cateter" sheetId="10" r:id="rId2"/>
-    <sheet name="CambioDeEstado" sheetId="9" r:id="rId3"/>
-    <sheet name="Historial1" sheetId="8" r:id="rId4"/>
-    <sheet name="Usuario" sheetId="7" r:id="rId5"/>
-    <sheet name="Cita" sheetId="5" r:id="rId6"/>
-    <sheet name="Paciente" sheetId="4" r:id="rId7"/>
-    <sheet name="Hemodialisis" sheetId="3" r:id="rId8"/>
-    <sheet name="Consulta" sheetId="6" r:id="rId9"/>
+    <sheet name="Paciente" sheetId="4" r:id="rId3"/>
+    <sheet name="Mortalidad" sheetId="11" r:id="rId4"/>
+    <sheet name="CambioDeEstado" sheetId="9" r:id="rId5"/>
+    <sheet name="Historial1" sheetId="8" r:id="rId6"/>
+    <sheet name="Usuario" sheetId="7" r:id="rId7"/>
+    <sheet name="Cita" sheetId="5" r:id="rId8"/>
+    <sheet name="Hemodialisis" sheetId="3" r:id="rId9"/>
+    <sheet name="Consulta" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="288">
   <si>
     <t>Paciente</t>
   </si>
@@ -604,15 +605,6 @@
      "cantidad": x,
      "mg": y
 }
-}</t>
-  </si>
-  <si>
-    <t>{
-	idConsulta:
-	{
-                idDoctor: x,
-                comentario: "comentario"
-	}	
 }</t>
   </si>
   <si>
@@ -984,12 +976,47 @@
   <si>
     <t>Indicacion JSON formato</t>
   </si>
+  <si>
+    <t>Entero</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Indicacion JSON CausaMuerte</t>
+  </si>
+  <si>
+    <t>CausaDeMuerte</t>
+  </si>
+  <si>
+    <t>DxAsociado</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Letra</t>
+  </si>
+  <si>
+    <t>VARCHAR(1)</t>
+  </si>
+  <si>
+    <t>"{
+	idConsulta:
+	{
+                idDoctor:{
+                	hora:["15:00","15:30"]
+                	comentario:["sada","daad"]
+                }
+	}	
+}"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1002,6 +1029,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1125,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1177,6 +1212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1489,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="L2:AS25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2:AG21"/>
+    <sheetView topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17:AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,38 +1563,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="12:44" x14ac:dyDescent="0.25">
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="P2" s="28" t="s">
+      <c r="M2" s="29"/>
+      <c r="P2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="Q2" s="30"/>
+      <c r="T2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="28"/>
-      <c r="AB2" s="25" t="s">
+      <c r="U2" s="30"/>
+      <c r="AB2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="25"/>
-      <c r="AF2" s="25" t="s">
+      <c r="AC2" s="27"/>
+      <c r="AF2" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="25"/>
-      <c r="AJ2" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK2" s="25"/>
-      <c r="AN2" s="25" t="s">
+      <c r="AG2" s="27"/>
+      <c r="AN2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="AO2" s="25"/>
-      <c r="AQ2" s="25" t="s">
+      <c r="AO2" s="27"/>
+      <c r="AQ2" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="AR2" s="25"/>
+      <c r="AR2" s="27"/>
     </row>
     <row r="3" spans="12:44" x14ac:dyDescent="0.25">
       <c r="L3" s="21" t="s">
@@ -1586,12 +1621,6 @@
         <v>1</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AN3" s="2" t="s">
@@ -1638,12 +1667,6 @@
       <c r="AG4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="AJ4" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="AN4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1688,12 +1711,6 @@
       <c r="AG5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AJ5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="AN5" s="6" t="s">
         <v>24</v>
       </c>
@@ -1738,12 +1755,6 @@
       <c r="AG6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AJ6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="AN6" s="8" t="s">
         <v>73</v>
       </c>
@@ -1764,22 +1775,16 @@
       <c r="AG7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="AJ7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="AN7" s="8" t="s">
         <v>74</v>
       </c>
       <c r="AO7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AQ7" s="25" t="s">
+      <c r="AQ7" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="AR7" s="25"/>
+      <c r="AR7" s="27"/>
     </row>
     <row r="8" spans="12:44" x14ac:dyDescent="0.25">
       <c r="AB8" s="6" t="s">
@@ -1794,12 +1799,6 @@
       <c r="AG8" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AJ8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK8" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="AN8" s="8" t="s">
         <v>75</v>
       </c>
@@ -1826,12 +1825,6 @@
       <c r="AG9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AJ9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK9" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="AN9" s="8" t="s">
         <v>76</v>
       </c>
@@ -1846,14 +1839,14 @@
       </c>
     </row>
     <row r="10" spans="12:44" x14ac:dyDescent="0.25">
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="Q10" s="25" t="s">
+      <c r="N10" s="27"/>
+      <c r="Q10" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="R10" s="25"/>
+      <c r="R10" s="27"/>
       <c r="AB10" s="6" t="s">
         <v>58</v>
       </c>
@@ -1892,10 +1885,10 @@
       <c r="R11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W11" s="25" t="s">
+      <c r="W11" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="X11" s="25"/>
+      <c r="X11" s="27"/>
       <c r="AB11" s="6" t="s">
         <v>59</v>
       </c>
@@ -1908,10 +1901,10 @@
       <c r="AG11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AI11" s="25" t="s">
+      <c r="AI11" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="AJ11" s="25"/>
+      <c r="AJ11" s="27"/>
       <c r="AN11" s="8" t="s">
         <v>78</v>
       </c>
@@ -2090,22 +2083,22 @@
       <c r="AG17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AI17" s="25" t="s">
+      <c r="AI17" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="AJ17" s="25"/>
-      <c r="AL17" s="25" t="s">
+      <c r="AJ17" s="27"/>
+      <c r="AL17" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="AM17" s="25"/>
-      <c r="AO17" s="25" t="s">
+      <c r="AM17" s="27"/>
+      <c r="AO17" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="AP17" s="25"/>
-      <c r="AR17" s="25" t="s">
+      <c r="AP17" s="27"/>
+      <c r="AR17" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="AS17" s="25"/>
+      <c r="AS17" s="27"/>
     </row>
     <row r="18" spans="17:45" x14ac:dyDescent="0.25">
       <c r="AB18" s="8" t="s">
@@ -2216,10 +2209,10 @@
       </c>
     </row>
     <row r="21" spans="17:45" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q21" s="25" t="s">
+      <c r="Q21" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="R21" s="25"/>
+      <c r="R21" s="27"/>
       <c r="AF21" s="8" t="s">
         <v>167</v>
       </c>
@@ -2234,18 +2227,18 @@
       <c r="R22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AI22" s="25" t="s">
+      <c r="AI22" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="AJ22" s="25"/>
-      <c r="AM22" s="25" t="s">
+      <c r="AJ22" s="27"/>
+      <c r="AM22" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="AN22" s="25"/>
-      <c r="AP22" s="25" t="s">
+      <c r="AN22" s="27"/>
+      <c r="AP22" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="AQ22" s="25"/>
+      <c r="AQ22" s="27"/>
     </row>
     <row r="23" spans="17:45" x14ac:dyDescent="0.25">
       <c r="AI23" s="2" t="s">
@@ -2308,7 +2301,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="AQ2:AR2"/>
     <mergeCell ref="AQ7:AR7"/>
     <mergeCell ref="AM22:AN22"/>
@@ -2324,7 +2317,6 @@
     <mergeCell ref="W11:X11"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="L2:M2"/>
@@ -2336,12 +2328,762 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F98DDE-15D8-49FA-8386-9B6AB2ACC876}">
+  <dimension ref="B2:N49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="E2" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="K2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="27"/>
+    </row>
+    <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="H12" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" s="27"/>
+      <c r="M12" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="180" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="M23" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M25" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M27" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M28" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M29" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M30" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M31" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M32" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M33" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M34" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M36" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M37" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M38" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M40" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M41" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M43" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M46" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M47" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E519D9-AC6E-4A7D-ACC1-2BD65084138B}">
   <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,10 +3094,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="C2" s="25"/>
+      <c r="B2" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
@@ -2365,18 +3107,18 @@
         <v>2</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -2384,15 +3126,15 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2400,7 +3142,7 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -2420,6 +3162,610 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B966206-6D01-4FB2-A1F1-B6F90191F93D}">
+  <dimension ref="B2:J30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="F2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="I2" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="I9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="27"/>
+      <c r="I14" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="I19" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41F415A-5F97-451A-9559-A2F5EB543900}">
+  <dimension ref="B2:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="E2" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185252DB-6684-4B99-86F4-E06202E9AFF1}">
   <dimension ref="B2:G8"/>
   <sheetViews>
@@ -2430,14 +3776,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -2461,7 +3807,7 @@
         <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
         <v>88</v>
@@ -2478,7 +3824,7 @@
         <v>165</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -2514,7 +3860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BE3169-7516-4FA7-BF44-04CFED4C374D}">
   <dimension ref="B2:F5"/>
   <sheetViews>
@@ -2528,10 +3874,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2552,12 +3898,12 @@
         <v>88</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
         <v>111</v>
@@ -2572,7 +3918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEA4641-8194-4D7E-91A0-D6203E3EE5DB}">
   <dimension ref="B2:C13"/>
   <sheetViews>
@@ -2586,10 +3932,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -2640,10 +3986,10 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -2678,7 +4024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7562A2-4896-4EC9-B58D-16DD9B74A1D0}">
   <dimension ref="B2:F9"/>
   <sheetViews>
@@ -2692,14 +4038,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="E2" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" s="25"/>
+      <c r="B2" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="E2" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
@@ -2717,13 +4063,13 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>88</v>
@@ -2731,7 +4077,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>88</v>
@@ -2745,7 +4091,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>88</v>
@@ -2756,20 +4102,20 @@
         <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>88</v>
@@ -2784,406 +4130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B966206-6D01-4FB2-A1F1-B6F90191F93D}">
-  <dimension ref="B2:J22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="F2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="25"/>
-      <c r="I2" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="25"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="29"/>
-      <c r="I9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="25"/>
-      <c r="I14" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="25"/>
-      <c r="I19" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="J19" s="25"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I7:J7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D5C14-7EB0-4720-97C9-161A5D908289}">
   <dimension ref="A1:P59"/>
   <sheetViews>
@@ -3200,28 +4147,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L1" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="L1" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="D2" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
+      <c r="A2" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="D2" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3236,20 +4183,20 @@
       <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N3" s="25"/>
+      <c r="M3" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>88</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>88</v>
@@ -3258,7 +4205,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3269,16 +4216,16 @@
         <v>91</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>88</v>
       </c>
       <c r="M5" t="s">
-        <v>209</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>215</v>
+        <v>208</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -3286,65 +4233,65 @@
         <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="N6" s="31"/>
+        <v>196</v>
+      </c>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="31"/>
+      <c r="N7" s="33"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N8" s="31"/>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="31"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="N10" s="31"/>
+      <c r="N10" s="33"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="33"/>
+      <c r="A11" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="35"/>
       <c r="D11" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>88</v>
@@ -3358,25 +4305,25 @@
         <v>2</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="M12" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N12" s="25"/>
+      <c r="M12" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="N12" s="27"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>88</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>88</v>
@@ -3385,7 +4332,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3396,85 +4343,85 @@
         <v>91</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>233</v>
-      </c>
       <c r="M14" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="N14" s="30" t="s">
-        <v>215</v>
+        <v>223</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D15" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N15" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N16" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N16" s="33"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N17" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N17" s="33"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D18" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="31"/>
+      <c r="N18" s="33"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" s="33"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="D20" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="N19" s="31"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="D20" s="20" t="s">
-        <v>239</v>
-      </c>
       <c r="E20" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3485,34 +4432,34 @@
         <v>2</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N21" s="25"/>
+        <v>232</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="N21" s="27"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>88</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M22" s="18" t="s">
         <v>1</v>
       </c>
       <c r="N22" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3523,99 +4470,99 @@
         <v>91</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>215</v>
+        <v>228</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N24" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>162</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N25" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N25" s="33"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="N26" s="31"/>
+        <v>232</v>
+      </c>
+      <c r="N26" s="33"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D27" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="N27" s="31"/>
+      <c r="N27" s="33"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="N28" s="31"/>
+      <c r="N28" s="33"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3623,16 +4570,16 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>250</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3640,22 +4587,22 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N31" s="25"/>
+        <v>232</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="N31" s="27"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D32" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>111</v>
@@ -3664,23 +4611,23 @@
         <v>1</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M33" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="N33" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="N33" s="30" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="B34" s="33"/>
-      <c r="N34" s="31"/>
+      <c r="A34" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="N34" s="33"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
@@ -3689,16 +4636,16 @@
       <c r="B35" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="31"/>
+      <c r="N35" s="33"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N36" s="31"/>
+      <c r="N36" s="33"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -3707,17 +4654,17 @@
       <c r="B37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N37" s="31"/>
+      <c r="N37" s="33"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="31"/>
+      <c r="N38" s="33"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3725,35 +4672,35 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
-      </c>
-      <c r="M40" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N40" s="25"/>
+        <v>222</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M41" s="18" t="s">
         <v>1</v>
       </c>
       <c r="N41" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M42" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="N42" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="N42" s="30" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="33"/>
-      <c r="N43" s="31"/>
+      <c r="A43" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="N43" s="33"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
@@ -3762,16 +4709,16 @@
       <c r="B44" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N44" s="31"/>
+      <c r="N44" s="33"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="31"/>
+      <c r="N45" s="33"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -3780,17 +4727,17 @@
       <c r="B46" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N46" s="31"/>
+      <c r="N46" s="33"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N47" s="31"/>
+      <c r="N47" s="33"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3798,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3806,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3814,14 +4761,14 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="35"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
@@ -3833,7 +4780,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>88</v>
@@ -3852,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3860,7 +4807,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3886,754 +4833,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F98DDE-15D8-49FA-8386-9B6AB2ACC876}">
-  <dimension ref="B2:N49"/>
-  <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="E2" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="25"/>
-      <c r="H2" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="I2" s="25"/>
-      <c r="K2" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="25"/>
-    </row>
-    <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="F12" s="25"/>
-      <c r="H12" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" s="25"/>
-      <c r="M12" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="M23" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M24" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M25" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M27" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M28" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M29" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M30" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M31" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M32" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M33" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M34" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M35" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M36" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M37" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="N37" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M38" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M39" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M40" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M41" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M42" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="N42" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M43" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="N43" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M44" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="N44" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M45" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N45" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M46" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N46" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N47" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M48" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="N48" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M49" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H12:I12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega La tabla transplante renal al diseño de la base de datos
</commit_message>
<xml_diff>
--- a/Diseño de base de datos/diseño.xlsx
+++ b/Diseño de base de datos/diseño.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303DB939-CBC2-4086-9545-77D782205F4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB128E54-53AD-4992-97C6-4AAF50C92541}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="655" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacional" sheetId="1" r:id="rId1"/>
     <sheet name="ReporteTransfusiones" sheetId="15" r:id="rId2"/>
-    <sheet name="Paciente" sheetId="4" r:id="rId3"/>
-    <sheet name="ReporteInfeccionAsociadoACatete" sheetId="13" r:id="rId4"/>
-    <sheet name="ReportePeritonitisOInfeccion" sheetId="14" r:id="rId5"/>
-    <sheet name="Cateter" sheetId="10" r:id="rId6"/>
-    <sheet name="Hemodialisis" sheetId="3" r:id="rId7"/>
-    <sheet name="Mortalidad" sheetId="11" r:id="rId8"/>
-    <sheet name="CambioDeEstado" sheetId="9" r:id="rId9"/>
-    <sheet name="Historial1" sheetId="8" r:id="rId10"/>
-    <sheet name="Usuario" sheetId="7" r:id="rId11"/>
-    <sheet name="Cita" sheetId="5" r:id="rId12"/>
-    <sheet name="Consulta" sheetId="6" r:id="rId13"/>
+    <sheet name="TransplanteRenal" sheetId="16" r:id="rId3"/>
+    <sheet name="Paciente" sheetId="4" r:id="rId4"/>
+    <sheet name="ReporteInfeccionAsociadoACatete" sheetId="13" r:id="rId5"/>
+    <sheet name="ReportePeritonitisOInfeccion" sheetId="14" r:id="rId6"/>
+    <sheet name="Cateter" sheetId="10" r:id="rId7"/>
+    <sheet name="Hemodialisis" sheetId="3" r:id="rId8"/>
+    <sheet name="Mortalidad" sheetId="11" r:id="rId9"/>
+    <sheet name="CambioDeEstado" sheetId="9" r:id="rId10"/>
+    <sheet name="Historial1" sheetId="8" r:id="rId11"/>
+    <sheet name="Usuario" sheetId="7" r:id="rId12"/>
+    <sheet name="Cita" sheetId="5" r:id="rId13"/>
+    <sheet name="Consulta" sheetId="6" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="338">
   <si>
     <t>Paciente</t>
   </si>
@@ -1136,6 +1137,33 @@
   </si>
   <si>
     <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>Transplante Renal</t>
+  </si>
+  <si>
+    <t>CausaERC</t>
+  </si>
+  <si>
+    <t>TipoDeDonante</t>
+  </si>
+  <si>
+    <t>TiemposDeIsquemia</t>
+  </si>
+  <si>
+    <t>CirugiaDeBanca</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>TransfusionesPrevias</t>
+  </si>
+  <si>
+    <t>ComplicacionesQuirurgicas</t>
+  </si>
+  <si>
+    <t>VARCHAR(120)</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1348,6 +1376,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1357,8 +1391,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1368,18 +1411,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1698,34 +1729,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="12:44" x14ac:dyDescent="0.25">
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="P2" s="31" t="s">
+      <c r="M2" s="34"/>
+      <c r="P2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="T2" s="31" t="s">
+      <c r="Q2" s="35"/>
+      <c r="T2" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="31"/>
-      <c r="AB2" s="28" t="s">
+      <c r="U2" s="35"/>
+      <c r="AB2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="28"/>
-      <c r="AF2" s="28" t="s">
+      <c r="AC2" s="32"/>
+      <c r="AF2" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="28"/>
-      <c r="AN2" s="28" t="s">
+      <c r="AG2" s="32"/>
+      <c r="AN2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AO2" s="28"/>
-      <c r="AQ2" s="28" t="s">
+      <c r="AO2" s="32"/>
+      <c r="AQ2" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="AR2" s="28"/>
+      <c r="AR2" s="32"/>
     </row>
     <row r="3" spans="12:44" x14ac:dyDescent="0.25">
       <c r="L3" s="21" t="s">
@@ -1916,10 +1947,10 @@
       <c r="AO7" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AQ7" s="28" t="s">
+      <c r="AQ7" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="AR7" s="28"/>
+      <c r="AR7" s="32"/>
     </row>
     <row r="8" spans="12:44" x14ac:dyDescent="0.25">
       <c r="AB8" s="6" t="s">
@@ -1974,14 +2005,14 @@
       </c>
     </row>
     <row r="10" spans="12:44" x14ac:dyDescent="0.25">
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="N10" s="28"/>
-      <c r="Q10" s="28" t="s">
+      <c r="N10" s="32"/>
+      <c r="Q10" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="R10" s="28"/>
+      <c r="R10" s="32"/>
       <c r="AB10" s="6" t="s">
         <v>58</v>
       </c>
@@ -2020,10 +2051,10 @@
       <c r="R11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W11" s="28" t="s">
+      <c r="W11" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="X11" s="28"/>
+      <c r="X11" s="32"/>
       <c r="AB11" s="6" t="s">
         <v>59</v>
       </c>
@@ -2036,10 +2067,10 @@
       <c r="AG11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AI11" s="28" t="s">
+      <c r="AI11" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="AJ11" s="28"/>
+      <c r="AJ11" s="32"/>
       <c r="AN11" s="8" t="s">
         <v>78</v>
       </c>
@@ -2218,22 +2249,22 @@
       <c r="AG17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AI17" s="28" t="s">
+      <c r="AI17" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="AJ17" s="28"/>
-      <c r="AL17" s="28" t="s">
+      <c r="AJ17" s="32"/>
+      <c r="AL17" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="AM17" s="28"/>
-      <c r="AO17" s="28" t="s">
+      <c r="AM17" s="32"/>
+      <c r="AO17" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="AP17" s="28"/>
-      <c r="AR17" s="28" t="s">
+      <c r="AP17" s="32"/>
+      <c r="AR17" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AS17" s="28"/>
+      <c r="AS17" s="32"/>
     </row>
     <row r="18" spans="17:45" x14ac:dyDescent="0.25">
       <c r="AB18" s="8" t="s">
@@ -2344,10 +2375,10 @@
       </c>
     </row>
     <row r="21" spans="17:45" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q21" s="28" t="s">
+      <c r="Q21" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="R21" s="28"/>
+      <c r="R21" s="32"/>
       <c r="AF21" s="8" t="s">
         <v>167</v>
       </c>
@@ -2362,18 +2393,18 @@
       <c r="R22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AI22" s="28" t="s">
+      <c r="AI22" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="AJ22" s="28"/>
-      <c r="AM22" s="28" t="s">
+      <c r="AJ22" s="32"/>
+      <c r="AM22" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="AN22" s="28"/>
-      <c r="AP22" s="28" t="s">
+      <c r="AN22" s="32"/>
+      <c r="AP22" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AQ22" s="28"/>
+      <c r="AQ22" s="32"/>
     </row>
     <row r="23" spans="17:45" x14ac:dyDescent="0.25">
       <c r="AI23" s="2" t="s">
@@ -2437,16 +2468,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="AI22:AJ22"/>
     <mergeCell ref="AQ2:AR2"/>
     <mergeCell ref="AQ7:AR7"/>
     <mergeCell ref="AM22:AN22"/>
@@ -2457,6 +2478,16 @@
     <mergeCell ref="AR17:AS17"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AI11:AJ11"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2464,6 +2495,101 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185252DB-6684-4B99-86F4-E06202E9AFF1}">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="F2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BE3169-7516-4FA7-BF44-04CFED4C374D}">
   <dimension ref="B2:F5"/>
   <sheetViews>
@@ -2477,10 +2603,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2521,7 +2647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEA4641-8194-4D7E-91A0-D6203E3EE5DB}">
   <dimension ref="B2:C13"/>
   <sheetViews>
@@ -2535,10 +2661,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -2589,10 +2715,10 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="32"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -2627,7 +2753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7562A2-4896-4EC9-B58D-16DD9B74A1D0}">
   <dimension ref="B2:F9"/>
   <sheetViews>
@@ -2641,14 +2767,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="E2" s="28" t="s">
+      <c r="C2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="F2" s="28"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
@@ -2733,7 +2859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F98DDE-15D8-49FA-8386-9B6AB2ACC876}">
   <dimension ref="B2:N49"/>
   <sheetViews>
@@ -2749,25 +2875,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="E2" s="28" t="s">
+      <c r="C2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="32"/>
       <c r="K2" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="N2" s="28"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -3013,14 +3139,14 @@
       <c r="C12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="H12" s="28" t="s">
+      <c r="F12" s="32"/>
+      <c r="H12" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="32"/>
       <c r="M12" s="6" t="s">
         <v>131</v>
       </c>
@@ -3487,8 +3613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1A940F-C3DC-4215-B235-932893A75A4B}">
   <dimension ref="B2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,17 +3625,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="32"/>
       <c r="F2" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="32" t="s">
         <v>325</v>
       </c>
-      <c r="K2" s="28"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
@@ -3574,7 +3700,7 @@
       <c r="B7" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="31" t="s">
         <v>324</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -3629,13 +3755,13 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
       <c r="H12" s="6" t="s">
         <v>302</v>
       </c>
@@ -3644,11 +3770,11 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
       <c r="H13" s="6" t="s">
         <v>303</v>
       </c>
@@ -3657,11 +3783,11 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
       <c r="H14" s="6" t="s">
         <v>304</v>
       </c>
@@ -3670,11 +3796,11 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
       <c r="H15" s="6" t="s">
         <v>306</v>
       </c>
@@ -3683,24 +3809,24 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="H16" s="38" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="H16" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="29" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3713,6 +3839,258 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EFB33F-4B1E-4E1F-80FC-B3EA1D6E191B}">
+  <dimension ref="B2:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="J2" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="32"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B966206-6D01-4FB2-A1F1-B6F90191F93D}">
   <dimension ref="B2:J30"/>
   <sheetViews>
@@ -3729,18 +4107,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="C2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="32"/>
+      <c r="I2" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -3823,10 +4201,10 @@
       <c r="C7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="28"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -3849,10 +4227,10 @@
       <c r="C9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="37"/>
       <c r="I9" s="7" t="s">
         <v>19</v>
       </c>
@@ -3941,10 +4319,10 @@
       <c r="C14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="32"/>
       <c r="I14" s="6" t="s">
         <v>179</v>
       </c>
@@ -4027,14 +4405,14 @@
       <c r="C19" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="I19" s="28" t="s">
+      <c r="G19" s="32"/>
+      <c r="I19" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -4097,10 +4475,10 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F25" s="25" t="s">
@@ -4166,7 +4544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6CB189-CA5A-43D8-923D-62314B71B6DC}">
   <dimension ref="B2:F16"/>
   <sheetViews>
@@ -4182,10 +4560,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="32"/>
       <c r="F2" s="10" t="s">
         <v>299</v>
       </c>
@@ -4298,10 +4676,10 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="29" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4314,7 +4692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC33E85-2ECB-4736-B8F9-E018C8F2E5F5}">
   <dimension ref="B2:G24"/>
   <sheetViews>
@@ -4331,14 +4709,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="C2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
@@ -4405,10 +4783,10 @@
       <c r="C8" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
@@ -4467,16 +4845,16 @@
       <c r="C13" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="29" t="s">
         <v>263</v>
       </c>
       <c r="F14" s="27" t="s">
@@ -4501,10 +4879,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="29" t="s">
         <v>263</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -4515,66 +4893,66 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="30" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="30" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4589,7 +4967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E519D9-AC6E-4A7D-ACC1-2BD65084138B}">
   <dimension ref="B2:I22"/>
   <sheetViews>
@@ -4605,10 +4983,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
@@ -4620,10 +4998,10 @@
       <c r="F3" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="37" t="s">
         <v>291</v>
       </c>
-      <c r="I3" s="32"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -4694,10 +5072,10 @@
       <c r="C8" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -4839,7 +5217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D5C14-7EB0-4720-97C9-161A5D908289}">
   <dimension ref="A1:P59"/>
   <sheetViews>
@@ -4856,28 +5234,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="D2" s="28" t="s">
+      <c r="B2" s="41"/>
+      <c r="D2" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="E2" s="32"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -4892,10 +5270,10 @@
       <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="N3" s="28"/>
+      <c r="N3" s="32"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -4933,7 +5311,7 @@
       <c r="M5" t="s">
         <v>208</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="38" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4944,7 +5322,7 @@
       <c r="E6" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="N6" s="37"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -4959,7 +5337,7 @@
       <c r="E7" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="37"/>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -4974,7 +5352,7 @@
       <c r="E8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N8" s="37"/>
+      <c r="N8" s="39"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="6" t="s">
@@ -4983,7 +5361,7 @@
       <c r="E9" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="37"/>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" s="20" t="s">
@@ -4992,13 +5370,13 @@
       <c r="E10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="N10" s="37"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="B11" s="34"/>
+      <c r="B11" s="41"/>
       <c r="D11" s="20" t="s">
         <v>220</v>
       </c>
@@ -5019,10 +5397,10 @@
       <c r="E12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="N12" s="28"/>
+      <c r="N12" s="32"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -5060,7 +5438,7 @@
       <c r="M14" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="38" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5071,7 +5449,7 @@
       <c r="E15" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N15" s="37"/>
+      <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -5086,7 +5464,7 @@
       <c r="E16" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N16" s="37"/>
+      <c r="N16" s="39"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -5101,7 +5479,7 @@
       <c r="E17" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N17" s="37"/>
+      <c r="N17" s="39"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D18" s="20" t="s">
@@ -5110,7 +5488,7 @@
       <c r="E18" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="37"/>
+      <c r="N18" s="39"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="20" t="s">
@@ -5119,13 +5497,13 @@
       <c r="E19" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="N19" s="37"/>
+      <c r="N19" s="39"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="41"/>
       <c r="D20" s="20" t="s">
         <v>238</v>
       </c>
@@ -5146,10 +5524,10 @@
       <c r="E21" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="M21" s="28" t="s">
+      <c r="M21" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="N21" s="28"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -5187,7 +5565,7 @@
       <c r="M23" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="N23" s="36" t="s">
+      <c r="N23" s="38" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5198,7 +5576,7 @@
       <c r="E24" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N24" s="37"/>
+      <c r="N24" s="39"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -5213,7 +5591,7 @@
       <c r="E25" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N25" s="37"/>
+      <c r="N25" s="39"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -5228,7 +5606,7 @@
       <c r="E26" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N26" s="37"/>
+      <c r="N26" s="39"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -5243,7 +5621,7 @@
       <c r="E27" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="N27" s="37"/>
+      <c r="N27" s="39"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -5258,7 +5636,7 @@
       <c r="E28" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="N28" s="37"/>
+      <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -5304,10 +5682,10 @@
       <c r="E31" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="M31" s="28" t="s">
+      <c r="M31" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="N31" s="28"/>
+      <c r="N31" s="32"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D32" s="20" t="s">
@@ -5327,16 +5705,16 @@
       <c r="M33" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="N33" s="36" t="s">
+      <c r="N33" s="38" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="N34" s="37"/>
+      <c r="B34" s="41"/>
+      <c r="N34" s="39"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
@@ -5345,7 +5723,7 @@
       <c r="B35" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="37"/>
+      <c r="N35" s="39"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -5354,7 +5732,7 @@
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N36" s="37"/>
+      <c r="N36" s="39"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -5363,10 +5741,10 @@
       <c r="B37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N37" s="37"/>
+      <c r="N37" s="39"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="37"/>
+      <c r="N38" s="39"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -5383,10 +5761,10 @@
       <c r="B40" t="s">
         <v>222</v>
       </c>
-      <c r="M40" s="28" t="s">
+      <c r="M40" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="N40" s="28"/>
+      <c r="N40" s="32"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M41" s="18" t="s">
@@ -5400,16 +5778,16 @@
       <c r="M42" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="N42" s="36" t="s">
+      <c r="N42" s="38" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="N43" s="37"/>
+      <c r="B43" s="41"/>
+      <c r="N43" s="39"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
@@ -5418,7 +5796,7 @@
       <c r="B44" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N44" s="37"/>
+      <c r="N44" s="39"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -5427,7 +5805,7 @@
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="37"/>
+      <c r="N45" s="39"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -5436,10 +5814,10 @@
       <c r="B46" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N46" s="37"/>
+      <c r="N46" s="39"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N47" s="37"/>
+      <c r="N47" s="39"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -5474,10 +5852,10 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="B53" s="34"/>
+      <c r="B53" s="41"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
@@ -5521,6 +5899,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="L1:P2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="N5:N10"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="N14:N19"/>
     <mergeCell ref="A53:B53"/>
@@ -5533,18 +5917,12 @@
     <mergeCell ref="N42:N47"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="L1:P2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="N5:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41F415A-5F97-451A-9559-A2F5EB543900}">
   <dimension ref="B2:H13"/>
   <sheetViews>
@@ -5561,14 +5939,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="E2" s="28" t="s">
+      <c r="C2" s="32"/>
+      <c r="E2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="28"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -5651,10 +6029,10 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E11" s="25" t="s">
@@ -5692,99 +6070,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185252DB-6684-4B99-86F4-E06202E9AFF1}">
-  <dimension ref="B2:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="F2" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>